<commit_message>
Update round filter to 1210 and add new data
</commit_message>
<xml_diff>
--- a/geocoded_cache_healthy.xlsx
+++ b/geocoded_cache_healthy.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5869"/>
+  <dimension ref="A1:C5884"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -76722,6 +76722,201 @@
         <v>127.453756958876</v>
       </c>
     </row>
+    <row r="5870">
+      <c r="A5870" t="inlineStr">
+        <is>
+          <t>대전 동구 동서대로 1689</t>
+        </is>
+      </c>
+      <c r="B5870" t="n">
+        <v>36.3503349793975</v>
+      </c>
+      <c r="C5870" t="n">
+        <v>127.436711042049</v>
+      </c>
+    </row>
+    <row r="5871">
+      <c r="A5871" t="inlineStr">
+        <is>
+          <t>경기 고양시 일산서구 일중로15번길 86</t>
+        </is>
+      </c>
+      <c r="B5871" t="n">
+        <v>37.6829544408687</v>
+      </c>
+      <c r="C5871" t="n">
+        <v>126.770150560953</v>
+      </c>
+    </row>
+    <row r="5872">
+      <c r="A5872" t="inlineStr">
+        <is>
+          <t>경기 남양주시 사릉로34번길 24</t>
+        </is>
+      </c>
+      <c r="B5872" t="n">
+        <v>37.636181102973</v>
+      </c>
+      <c r="C5872" t="n">
+        <v>127.211071007036</v>
+      </c>
+    </row>
+    <row r="5873">
+      <c r="A5873" t="inlineStr">
+        <is>
+          <t>경기 수원시 장안구 팔달로 255</t>
+        </is>
+      </c>
+      <c r="B5873" t="n">
+        <v>37.2888295580437</v>
+      </c>
+      <c r="C5873" t="n">
+        <v>127.012935153781</v>
+      </c>
+    </row>
+    <row r="5874">
+      <c r="A5874" t="inlineStr">
+        <is>
+          <t>경기 파주시 방촌로 661</t>
+        </is>
+      </c>
+      <c r="B5874" t="n">
+        <v>37.8032911664257</v>
+      </c>
+      <c r="C5874" t="n">
+        <v>126.718263589781</v>
+      </c>
+    </row>
+    <row r="5875">
+      <c r="A5875" t="inlineStr">
+        <is>
+          <t>전남 강진군 중앙로 83</t>
+        </is>
+      </c>
+      <c r="B5875" t="n">
+        <v>34.6379301337033</v>
+      </c>
+      <c r="C5875" t="n">
+        <v>126.766631813094</v>
+      </c>
+    </row>
+    <row r="5876">
+      <c r="A5876" t="inlineStr">
+        <is>
+          <t>경남 김해시 장유로 288</t>
+        </is>
+      </c>
+      <c r="B5876" t="n">
+        <v>35.200014582908</v>
+      </c>
+      <c r="C5876" t="n">
+        <v>128.813796211671</v>
+      </c>
+    </row>
+    <row r="5877">
+      <c r="A5877" t="inlineStr">
+        <is>
+          <t>경남 창원시 성산구 원이대로 320</t>
+        </is>
+      </c>
+      <c r="B5877" t="n">
+        <v>35.2396668440149</v>
+      </c>
+      <c r="C5877" t="n">
+        <v>128.654408692296</v>
+      </c>
+    </row>
+    <row r="5878">
+      <c r="A5878" t="inlineStr">
+        <is>
+          <t>경기 남양주시 금강로 1557</t>
+        </is>
+      </c>
+      <c r="B5878" t="n">
+        <v>37.7297611357089</v>
+      </c>
+      <c r="C5878" t="n">
+        <v>127.192978788045</v>
+      </c>
+    </row>
+    <row r="5879">
+      <c r="A5879" t="inlineStr">
+        <is>
+          <t>서울 구로구 경인로35길 83</t>
+        </is>
+      </c>
+      <c r="B5879" t="n">
+        <v>37.5001514232447</v>
+      </c>
+      <c r="C5879" t="n">
+        <v>126.852353214482</v>
+      </c>
+    </row>
+    <row r="5880">
+      <c r="A5880" t="inlineStr">
+        <is>
+          <t>서울 은평구 연서로 9</t>
+        </is>
+      </c>
+      <c r="B5880" t="n">
+        <v>37.6000995302827</v>
+      </c>
+      <c r="C5880" t="n">
+        <v>126.91556845327</v>
+      </c>
+    </row>
+    <row r="5881">
+      <c r="A5881" t="inlineStr">
+        <is>
+          <t>인천 서구 심곡로49번길 2</t>
+        </is>
+      </c>
+      <c r="B5881" t="n">
+        <v>37.542334111634</v>
+      </c>
+      <c r="C5881" t="n">
+        <v>126.675314305948</v>
+      </c>
+    </row>
+    <row r="5882">
+      <c r="A5882" t="inlineStr">
+        <is>
+          <t>경기 구리시 경춘로 239</t>
+        </is>
+      </c>
+      <c r="B5882" t="n">
+        <v>37.6016291279841</v>
+      </c>
+      <c r="C5882" t="n">
+        <v>127.141642278598</v>
+      </c>
+    </row>
+    <row r="5883">
+      <c r="A5883" t="inlineStr">
+        <is>
+          <t>경기 안산시 단원구 원선1로 38</t>
+        </is>
+      </c>
+      <c r="B5883" t="n">
+        <v>37.326166138141</v>
+      </c>
+      <c r="C5883" t="n">
+        <v>126.803777208185</v>
+      </c>
+    </row>
+    <row r="5884">
+      <c r="A5884" t="inlineStr">
+        <is>
+          <t>경북 문경시 중앙로 156</t>
+        </is>
+      </c>
+      <c r="B5884" t="n">
+        <v>36.5984046449212</v>
+      </c>
+      <c r="C5884" t="n">
+        <v>128.201837051878</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update: Registered 131/270 shops and Round 1211 emergency data update with scraper fix
</commit_message>
<xml_diff>
--- a/geocoded_cache_healthy.xlsx
+++ b/geocoded_cache_healthy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5884"/>
+  <dimension ref="A1:C5891"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -76917,6 +76917,97 @@
         <v>128.201837051878</v>
       </c>
     </row>
+    <row r="5885">
+      <c r="A5885" t="inlineStr">
+        <is>
+          <t>서울 중구 청파로 451-1</t>
+        </is>
+      </c>
+      <c r="B5885" t="n">
+        <v>37.559632141397</v>
+      </c>
+      <c r="C5885" t="n">
+        <v>126.968098154883</v>
+      </c>
+    </row>
+    <row r="5886">
+      <c r="A5886" t="inlineStr">
+        <is>
+          <t>광주 서구 상무대로 871 1층(쌍촌동)</t>
+        </is>
+      </c>
+      <c r="B5886" t="n">
+        <v>35.1505172187205</v>
+      </c>
+      <c r="C5886" t="n">
+        <v>126.857294259506</v>
+      </c>
+    </row>
+    <row r="5887">
+      <c r="A5887" t="inlineStr">
+        <is>
+          <t>경기 수원시 장안구 송원로 13 1층(송죽동)</t>
+        </is>
+      </c>
+      <c r="B5887" t="n">
+        <v>37.2971375341087</v>
+      </c>
+      <c r="C5887" t="n">
+        <v>127.00529752128</v>
+      </c>
+    </row>
+    <row r="5888">
+      <c r="A5888" t="inlineStr">
+        <is>
+          <t>경기 용인시 기흥구 구성3로28번길 12 101호</t>
+        </is>
+      </c>
+      <c r="B5888" t="n">
+        <v>37.2946064718643</v>
+      </c>
+      <c r="C5888" t="n">
+        <v>127.151765073871</v>
+      </c>
+    </row>
+    <row r="5889">
+      <c r="A5889" t="inlineStr">
+        <is>
+          <t>경기 화성시 푸른들판로 660</t>
+        </is>
+      </c>
+      <c r="B5889" t="n">
+        <v>37.1674665832359</v>
+      </c>
+      <c r="C5889" t="n">
+        <v>126.895690863305</v>
+      </c>
+    </row>
+    <row r="5890">
+      <c r="A5890" t="inlineStr">
+        <is>
+          <t>경남 거제시 장승포로 11</t>
+        </is>
+      </c>
+      <c r="B5890" t="n">
+        <v>34.8678721675344</v>
+      </c>
+      <c r="C5890" t="n">
+        <v>128.725345701113</v>
+      </c>
+    </row>
+    <row r="5891">
+      <c r="A5891" t="inlineStr">
+        <is>
+          <t>경남 양산시 상북중앙로 319</t>
+        </is>
+      </c>
+      <c r="B5891" t="n">
+        <v>35.4121895785582</v>
+      </c>
+      <c r="C5891" t="n">
+        <v>129.059189941123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>